<commit_message>
New Timetables and faculty details added
</commit_message>
<xml_diff>
--- a/Modified Data/EEE1.xlsx
+++ b/Modified Data/EEE1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\ABHISHEK ARANGI\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VLSID\Mukesh\Time_Table_Management_Using_GenAI\Modified Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7852E9-F30E-4159-B6DE-5271A476ECBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B5DFD4-8CE4-4ED8-B240-0F168A34E66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="103">
   <si>
     <t>E1</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>23PY1102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECT GUIDE </t>
   </si>
 </sst>
 </file>
@@ -605,73 +608,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -681,25 +638,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -710,47 +655,105 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1031,15 +1034,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DABB36-FA05-4FE1-95A0-F7875285AF03}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="61" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="36" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1050,17 +1053,17 @@
       <c r="B1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="12" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1068,20 +1071,20 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="31" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1089,20 +1092,20 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="31" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1110,20 +1113,20 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="31" t="s">
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1131,20 +1134,20 @@
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="31" t="s">
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1152,20 +1155,20 @@
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="31" t="s">
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1173,20 +1176,20 @@
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="31" t="s">
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1194,20 +1197,20 @@
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="31" t="s">
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1215,20 +1218,20 @@
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="31" t="s">
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1236,20 +1239,20 @@
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="12" t="s">
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1257,20 +1260,20 @@
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="12" t="s">
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1278,20 +1281,20 @@
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="30" t="s">
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1299,20 +1302,20 @@
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="12" t="s">
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="8" t="s">
         <v>43</v>
       </c>
       <c r="J13" s="1"/>
@@ -1321,125 +1324,125 @@
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="30" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="12" t="s">
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="39" customFormat="1" ht="15.75" thickBot="1">
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="21" customFormat="1" ht="15.75" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="30" t="s">
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="41" t="s">
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="40" t="s">
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="22" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1447,20 +1450,20 @@
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="30" t="s">
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1468,20 +1471,20 @@
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="30" t="s">
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1489,20 +1492,20 @@
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="12" t="s">
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1510,20 +1513,20 @@
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="12" t="s">
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1531,20 +1534,20 @@
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="30" t="s">
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1552,20 +1555,20 @@
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="30" t="s">
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1573,20 +1576,20 @@
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="40" t="s">
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="22" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1594,20 +1597,20 @@
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="30" t="s">
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="14" t="s">
         <v>43</v>
       </c>
       <c r="L27" s="1"/>
@@ -1616,20 +1619,20 @@
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="41" t="s">
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1637,20 +1640,20 @@
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="40" t="s">
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="22" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1658,20 +1661,20 @@
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="30" t="s">
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1679,20 +1682,20 @@
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="30" t="s">
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1700,20 +1703,20 @@
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C32" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="12" t="s">
+      <c r="E32" s="55"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="8" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1721,20 +1724,20 @@
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="12" t="s">
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1742,20 +1745,20 @@
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C34" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="30" t="s">
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1763,20 +1766,20 @@
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="30" t="s">
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1784,20 +1787,20 @@
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C36" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="30" t="s">
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="14" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1805,438 +1808,442 @@
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="54" t="s">
+      <c r="C37" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="30" t="s">
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="54" t="s">
+      <c r="C38" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="41" t="s">
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="54" t="s">
+      <c r="C39" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="40" t="s">
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="30" t="s">
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="57" t="s">
+      <c r="C41" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="30" t="s">
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="12" t="s">
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A43" s="45" t="s">
+      <c r="A43" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="47" t="s">
+      <c r="B43" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="57" t="s">
+      <c r="C43" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="12" t="s">
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="47" t="s">
+      <c r="B44" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="57" t="s">
+      <c r="C44" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="48" t="s">
+      <c r="D44" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="30" t="s">
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="B45" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="57" t="s">
+      <c r="C45" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="48" t="s">
+      <c r="D45" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="49"/>
-      <c r="I45" s="30" t="s">
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="57" t="s">
+      <c r="C46" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="48" t="s">
+      <c r="D46" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="49"/>
-      <c r="I46" s="30" t="s">
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="47" t="s">
+      <c r="B47" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="57" t="s">
+      <c r="C47" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="48" t="s">
+      <c r="D47" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="30" t="s">
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="47" t="s">
+      <c r="B48" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="57" t="s">
+      <c r="C48" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="48" t="s">
+      <c r="D48" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="49"/>
-      <c r="I48" s="41" t="s">
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="47" t="s">
+      <c r="B49" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="57" t="s">
+      <c r="C49" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="48" t="s">
+      <c r="D49" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="40" t="s">
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="22" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="47" t="s">
+      <c r="B50" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="57" t="s">
+      <c r="C50" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="48" t="s">
+      <c r="D50" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="30" t="s">
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="14" t="s">
         <v>41</v>
       </c>
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="47" t="s">
+      <c r="B51" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="57" t="s">
+      <c r="C51" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="48" t="s">
+      <c r="D51" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="49"/>
-      <c r="I51" s="30" t="s">
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="14" t="s">
         <v>43</v>
       </c>
       <c r="L51" s="1"/>
     </row>
     <row r="52" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="47" t="s">
+      <c r="B52" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="57" t="s">
+      <c r="C52" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="48" t="s">
+      <c r="D52" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="49"/>
-      <c r="I52" s="12" t="s">
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="47" t="s">
+      <c r="B53" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="57" t="s">
+      <c r="C53" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D53" s="48" t="s">
+      <c r="D53" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="49"/>
-      <c r="I53" s="12" t="s">
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="47" t="s">
+      <c r="B54" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="57" t="s">
+      <c r="C54" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D54" s="50"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="51"/>
-      <c r="I54" s="30" t="s">
+      <c r="D54" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="47" t="s">
+      <c r="B55" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C55" s="57" t="s">
+      <c r="C55" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D55" s="52"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="30" t="s">
+      <c r="D55" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="60"/>
+      <c r="I55" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B56" s="47" t="s">
+      <c r="B56" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C56" s="58" t="s">
+      <c r="C56" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="30" t="s">
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="47" t="s">
+      <c r="B57" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="58" t="s">
+      <c r="C57" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="30" t="s">
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2244,20 +2251,20 @@
       <c r="A58" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="59" t="s">
+      <c r="C58" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="18" t="s">
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2265,20 +2272,20 @@
       <c r="A59" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C59" s="60" t="s">
+      <c r="C59" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="21" t="s">
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="13" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2286,20 +2293,20 @@
       <c r="A60" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C60" s="57" t="s">
+      <c r="C60" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="18" t="s">
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2307,20 +2314,20 @@
       <c r="A61" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C61" s="57" t="s">
+      <c r="C61" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="17" t="s">
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="10" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2328,35 +2335,54 @@
       <c r="A62" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="57" t="s">
+      <c r="C62" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-      <c r="I62" s="21" t="s">
+      <c r="D62" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="13" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="D45:H45"/>
-    <mergeCell ref="D47:H47"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D25:H25"/>
+  <mergeCells count="62">
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D32:H32"/>
     <mergeCell ref="D59:H59"/>
     <mergeCell ref="D60:H60"/>
     <mergeCell ref="D61:H61"/>
@@ -2368,6 +2394,13 @@
     <mergeCell ref="D57:H57"/>
     <mergeCell ref="D58:H58"/>
     <mergeCell ref="D53:H53"/>
+    <mergeCell ref="D51:H51"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D25:H25"/>
     <mergeCell ref="D42:H42"/>
     <mergeCell ref="D44:H44"/>
     <mergeCell ref="D46:H46"/>
@@ -2377,35 +2410,12 @@
     <mergeCell ref="D37:H37"/>
     <mergeCell ref="D38:H38"/>
     <mergeCell ref="D40:H40"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="D45:H45"/>
+    <mergeCell ref="D47:H47"/>
     <mergeCell ref="D41:H41"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D5:H5"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>